<commit_message>
All Stock Parts Balanced (woo hoo, beer time!)
</commit_message>
<xml_diff>
--- a/KSP Universal Storage 2.xlsx
+++ b/KSP Universal Storage 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulK\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Kerbal Space Program 1.4 Making History\GameData\UniversalStorage2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67F6C5E-67CC-476E-9B4C-FB6172F4A270}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D452CBBC-03B6-4B2D-B8A7-C990838C5965}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="10590" windowHeight="12030" activeTab="1" xr2:uid="{C3245EDE-D602-4B47-9FA3-AA7BA4BF5217}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="10590" windowHeight="12030" xr2:uid="{C3245EDE-D602-4B47-9FA3-AA7BA4BF5217}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Mods list" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
   <si>
     <t>Stock</t>
   </si>
@@ -160,18 +160,12 @@
     <t>Mechjeb</t>
   </si>
   <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
     <t># Wedges</t>
   </si>
   <si>
-    <t>Weight PW</t>
-  </si>
-  <si>
     <t>Cost PW</t>
   </si>
   <si>
@@ -224,6 +218,120 @@
   </si>
   <si>
     <t>Structure</t>
+  </si>
+  <si>
+    <t>Wedge</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>EP Cost</t>
+  </si>
+  <si>
+    <t>Avarage structural mass per wedge</t>
+  </si>
+  <si>
+    <t>Avarage structural cost per wedge</t>
+  </si>
+  <si>
+    <t>Equivalent Part (EP)</t>
+  </si>
+  <si>
+    <t>Liquid Fuel / Ox</t>
+  </si>
+  <si>
+    <t>Electric Charge</t>
+  </si>
+  <si>
+    <t>Carbon Dioxide</t>
+  </si>
+  <si>
+    <t>Monoprop</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>EP Ratio</t>
+  </si>
+  <si>
+    <t>FL-T100</t>
+  </si>
+  <si>
+    <t>Wedge Cost</t>
+  </si>
+  <si>
+    <t>EP Mass</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Wedge Mass</t>
+  </si>
+  <si>
+    <t>Mass PW</t>
+  </si>
+  <si>
+    <t>Mass overhead</t>
+  </si>
+  <si>
+    <t>Cost overhead</t>
+  </si>
+  <si>
+    <t>Tot</t>
+  </si>
+  <si>
+    <t>Mass + OH</t>
+  </si>
+  <si>
+    <t>Cost + OH</t>
+  </si>
+  <si>
+    <t>FL-R25</t>
+  </si>
+  <si>
+    <t>Way too complex and doesn't really add up.  Feels like Epicycles</t>
+  </si>
+  <si>
+    <t>EMPW</t>
+  </si>
+  <si>
+    <t>ECPW</t>
+  </si>
+  <si>
+    <t>EMPW = Equivilent Mass Per Wedge, ECPW = Equivilent Cost Per Wedge</t>
+  </si>
+  <si>
+    <t>Mass with Structure</t>
+  </si>
+  <si>
+    <t>Cost with Structure</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Life Support Container (TAC)</t>
+  </si>
+  <si>
+    <t>Z-1K</t>
+  </si>
+  <si>
+    <t>TACLS Sabatier (TAC)</t>
+  </si>
+  <si>
+    <t>TACLS Water Purifier (TAC)</t>
+  </si>
+  <si>
+    <t>Aerozine</t>
   </si>
 </sst>
 </file>
@@ -233,7 +341,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,8 +424,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,8 +481,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -469,8 +602,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -479,8 +643,9 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1"/>
@@ -519,9 +684,48 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="2" xfId="7" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="6" fillId="7" borderId="1" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="3" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="8" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="6" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="6" xfId="6" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="6" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="7" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
+    <cellStyle name="Accent2" xfId="8" builtinId="33"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -530,7 +734,258 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="7" builtinId="21"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="25">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F76"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF7F7F7F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F76"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF7F7F7F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F76"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF7F7F7F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F76"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF7F7F7F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF7F7F7F"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -543,17 +998,14 @@
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
       <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -633,7 +1085,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Cost and weight should be ballanced on</a:t>
+            <a:t>Cost and weight should be balanced on</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
@@ -657,6 +1109,15 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>Hexa and Octo cores have additional C&amp;W to allow for crew transfer tunnel.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Mass is in 1000Kg (0.001 = 1Kg)</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -671,10 +1132,10 @@
   <autoFilter ref="A9:F15" xr:uid="{E35C78EA-37D4-4ED3-9810-2F527211F7B1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A579DE4B-A322-4B2E-9837-103820C03232}" name="Part"/>
-    <tableColumn id="2" xr3:uid="{BDEA9424-295C-438D-BC3E-B712CD75D492}" name="Weight" dataDxfId="3" dataCellStyle="Input"/>
-    <tableColumn id="3" xr3:uid="{BEC8C509-96C0-4C1D-B987-D949FCD72522}" name="Cost" dataDxfId="2" dataCellStyle="Input"/>
+    <tableColumn id="2" xr3:uid="{BDEA9424-295C-438D-BC3E-B712CD75D492}" name="Mass" dataDxfId="24" dataCellStyle="Input"/>
+    <tableColumn id="3" xr3:uid="{BEC8C509-96C0-4C1D-B987-D949FCD72522}" name="Cost" dataDxfId="23" dataCellStyle="Input"/>
     <tableColumn id="4" xr3:uid="{2CDA1B83-518F-4FCE-B239-152F6AAB9B0E}" name="# Wedges"/>
-    <tableColumn id="5" xr3:uid="{D72B8143-BCE8-4CA0-92EB-4F25A654E009}" name="Weight PW" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{D72B8143-BCE8-4CA0-92EB-4F25A654E009}" name="Mass PW" dataDxfId="22">
       <calculatedColumnFormula>B10/D10</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{7C548BED-B2C0-48CA-8E75-2EE5E27D006C}" name="Cost PW">
@@ -690,13 +1151,81 @@
   <autoFilter ref="A17:F20" xr:uid="{15374C48-326D-4B9F-89C7-9290C4904D94}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EFC3A571-8606-4D34-9570-444E46172573}" name="Assembly" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{39B14A51-C030-4BF0-976E-6004D7CB7614}" name="Weight" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{39B14A51-C030-4BF0-976E-6004D7CB7614}" name="Mass" dataDxfId="21" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{3085B6D2-8BD9-412D-9BB4-B061501AA3F5}" name="Cost" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{8AE4EF62-BE12-431E-8941-09FFEC2F04B1}" name="Column1" dataDxfId="0" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{07D0FC5F-9407-45B3-B1CF-2DA7FFBD07ED}" name="Weight PW" dataDxfId="1" dataCellStyle="Output"/>
+    <tableColumn id="4" xr3:uid="{8AE4EF62-BE12-431E-8941-09FFEC2F04B1}" name="Column1" dataDxfId="20" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{07D0FC5F-9407-45B3-B1CF-2DA7FFBD07ED}" name="Mass PW" dataDxfId="19" dataCellStyle="Output"/>
     <tableColumn id="6" xr3:uid="{EAED86FD-9C2D-43A3-8AED-2A35A4B0E8C1}" name="Cost PW" dataCellStyle="Output"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3D0D9A4A-463F-4D26-82AA-63A5B0C8CC4F}" name="Table3" displayName="Table3" ref="J9:W24" totalsRowShown="0">
+  <autoFilter ref="J9:W24" xr:uid="{FCFFE02D-0F9D-47CE-8963-D0B96401028F}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{D35C5EED-7BD1-4643-8282-F63E139564EA}" name="Wedge"/>
+    <tableColumn id="6" xr3:uid="{8634F600-D183-4F35-9174-CF6AFDB437E9}" name="Resource"/>
+    <tableColumn id="7" xr3:uid="{36D05634-ED80-4A39-A2B6-D12AE024D880}" name="Equivalent Part (EP)" dataCellStyle="Input"/>
+    <tableColumn id="8" xr3:uid="{3E6D94E4-6CE3-49EC-B2D7-CDEF9031A5D1}" name="EP Mass" dataDxfId="18" dataCellStyle="Input"/>
+    <tableColumn id="9" xr3:uid="{DB2B2C2C-9933-42E8-A081-7B51720E5BAE}" name="EP Cost" dataCellStyle="Input"/>
+    <tableColumn id="10" xr3:uid="{7E87F25C-5A4C-4DF5-A29D-200B2970A86E}" name="EP Ratio" dataCellStyle="Input"/>
+    <tableColumn id="2" xr3:uid="{76FFECEC-42C1-4853-B453-CD67BCEA4C82}" name="EMPW" dataDxfId="17">
+      <calculatedColumnFormula>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{6648A9CF-A240-4F40-9B6F-7036BFC6FDF0}" name="ECPW" dataDxfId="16">
+      <calculatedColumnFormula>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{335079E6-1470-4AD7-8DAE-D5030809B2E3}" name="Wedge Mass" dataDxfId="15">
+      <calculatedColumnFormula>Table3[[#This Row],[EMPW]]-$F$4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{99B210F1-A8A3-43A7-8333-E8BB85F0B547}" name="Wedge Cost" dataDxfId="14">
+      <calculatedColumnFormula>Table3[[#This Row],[ECPW]]-$F$5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{404FE096-C0F6-4430-B9AE-0C0079420A1E}" name="Mass + OH" dataDxfId="13">
+      <calculatedColumnFormula>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{3E12FB57-74FA-4B05-ADFF-6CCFD7C06427}" name="Cost + OH" dataDxfId="12">
+      <calculatedColumnFormula>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{59A654E4-65C3-446D-8823-21A7DAD93D58}" name="Mass with Structure" dataDxfId="11" dataCellStyle="Output">
+      <calculatedColumnFormula>Table3[[#This Row],[Mass + OH]]+$F$4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{F355FCD9-68F4-49E3-835F-663E86D3B79B}" name="Cost with Structure" dataDxfId="10" dataCellStyle="Output">
+      <calculatedColumnFormula>Table3[[#This Row],[Cost + OH]]+$F$5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B3A231BC-39A7-4EE7-9404-BCFF8A0EB73D}" name="Table4" displayName="Table4" ref="J28:U43" totalsRowShown="0">
+  <autoFilter ref="J28:U43" xr:uid="{46081FD9-DEF6-425C-B392-40ECBEDC37F3}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{3A5AB019-9F60-4DA4-846C-B79D4002996A}" name="Wedge" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{029965FB-BA4B-48F3-871C-0C2DCB8A6561}" name="Resource" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{038C1B73-CADE-41CD-B1C1-05FF0A2BE1CE}" name="Equivalent Part (EP)" dataDxfId="7" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{FD0E5793-2888-43BB-930B-A5077DC78A62}" name="EP Mass" dataDxfId="6" dataCellStyle="Input"/>
+    <tableColumn id="5" xr3:uid="{52F5C845-80EC-431F-8212-494C84B32728}" name="EP Cost" dataDxfId="5" dataCellStyle="Input"/>
+    <tableColumn id="6" xr3:uid="{AF154CBF-F54F-4E51-8889-F4DB73C16004}" name="EP Ratio" dataDxfId="4" dataCellStyle="Input"/>
+    <tableColumn id="7" xr3:uid="{6B1F7D26-131C-42E1-ABAF-EE8782299855}" name="EMPW" dataDxfId="3" dataCellStyle="Normal">
+      <calculatedColumnFormula>M29/O29</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{B407898F-3ADA-4E54-ADDC-5EADD291509F}" name="ECPW" dataDxfId="2" dataCellStyle="Normal">
+      <calculatedColumnFormula>N29/O29</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{3F4CC5AE-B283-42BA-AA44-9D8055720245}" name="Column1"/>
+    <tableColumn id="10" xr3:uid="{D9EFCA45-4D60-400B-AD7E-7C4B507FFC94}" name="Column2"/>
+    <tableColumn id="11" xr3:uid="{CED7D517-BD40-498E-AA55-203E544DE2AF}" name="Wedge Mass" dataDxfId="0">
+      <calculatedColumnFormula>Table4[[#This Row],[EMPW]]-$F$4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{37C9ED97-13F9-4DEF-BFA8-5B6D153D7855}" name="Wedge Cost" dataDxfId="1">
+      <calculatedColumnFormula>Table4[[#This Row],[ECPW]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -999,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A844A3D-DE41-49C6-9CA4-260D9D9B0D6E}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1612,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -1111,7 +1640,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J5" t="s">
         <v>32</v>
@@ -1122,84 +1651,92 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,6 +1745,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:A23">
+    <sortCondition ref="A23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1215,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1933BA2C-6D76-4E2A-A0F4-C7FFE13A3365}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,57 +1768,143 @@
     <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="14" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="19" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:23" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="8">
+        <f>AVERAGE(Table2[Mass PW])</f>
+        <v>1.0972222222222222E-2</v>
+      </c>
+      <c r="V4" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="32">
+        <f>AVERAGE(Table2[Cost PW])</f>
+        <v>59.166666666666664</v>
+      </c>
+      <c r="V5" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="W5" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="W8" s="55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="K9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="L9" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="N9" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="P9" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q9" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="R9" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="S9" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="T9" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="U9" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="V9" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="W9" s="54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>49</v>
       </c>
       <c r="B10" s="16">
         <v>0.02</v>
@@ -1297,10 +1923,60 @@
         <f>C10/D10</f>
         <v>31.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="45">
+        <v>6.3E-2</v>
+      </c>
+      <c r="N10" s="44">
+        <v>150</v>
+      </c>
+      <c r="O10" s="44">
+        <v>4</v>
+      </c>
+      <c r="P10" s="7">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>1.575E-2</v>
+      </c>
+      <c r="Q10" s="31">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>37.5</v>
+      </c>
+      <c r="R10" s="7">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>4.7777777777777784E-3</v>
+      </c>
+      <c r="S10" s="31">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>-21.666666666666664</v>
+      </c>
+      <c r="T10" s="7">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>1.0263888888888888E-2</v>
+      </c>
+      <c r="U10" s="31">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>-21.661180555555553</v>
+      </c>
+      <c r="V10" s="12">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>2.1236111111111108E-2</v>
+      </c>
+      <c r="W10" s="38">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>37.505486111111111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="18">
         <v>0.01</v>
@@ -1319,10 +1995,58 @@
         <f t="shared" ref="F11:F15" si="1">C11/D11</f>
         <v>21.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="15"/>
+      <c r="M11" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="N11" s="15">
+        <v>880</v>
+      </c>
+      <c r="O11" s="15">
+        <v>2</v>
+      </c>
+      <c r="P11" s="7">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Q11" s="31">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>440</v>
+      </c>
+      <c r="R11" s="7">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>1.402777777777778E-2</v>
+      </c>
+      <c r="S11" s="31">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>380.83333333333331</v>
+      </c>
+      <c r="T11" s="7">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>1.951388888888889E-2</v>
+      </c>
+      <c r="U11" s="31">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>380.83881944444443</v>
+      </c>
+      <c r="V11" s="8">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>3.048611111111111E-2</v>
+      </c>
+      <c r="W11" s="32">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>440.00548611111111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="18">
         <v>0.05</v>
@@ -1341,10 +2065,52 @@
         <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" s="15"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q12" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R12" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S12" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T12" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U12" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V12" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W12" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="18">
         <v>0.125</v>
@@ -1363,10 +2129,49 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="15"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q13" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R13" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S13" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T13" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U13" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V13" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W13" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B14" s="18">
         <v>7.4999999999999997E-2</v>
@@ -1385,10 +2190,49 @@
         <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="15"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q14" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S14" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T14" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U14" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V14" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W14" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" s="20">
         <v>0.02</v>
@@ -1407,30 +2251,149 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="15"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q15" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R15" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S15" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T15" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U15" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V15" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W15" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="15"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q16" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R16" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S16" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T16" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U16" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V16" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W16" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
       <c r="D17" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="J17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="15"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q17" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R17" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S17" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T17" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U17" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V17" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W17" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="7">
         <f>B11+B10</f>
@@ -1449,10 +2412,60 @@
         <f>F11+F10</f>
         <v>52.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="M18" s="39">
+        <v>0.8</v>
+      </c>
+      <c r="N18" s="15">
+        <v>330</v>
+      </c>
+      <c r="O18" s="15">
+        <v>4</v>
+      </c>
+      <c r="P18" s="7">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q18" s="31">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>82.5</v>
+      </c>
+      <c r="R18" s="7">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>0.18902777777777779</v>
+      </c>
+      <c r="S18" s="31">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>23.333333333333336</v>
+      </c>
+      <c r="T18" s="7">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>0.1945138888888889</v>
+      </c>
+      <c r="U18" s="31">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>23.338819444444447</v>
+      </c>
+      <c r="V18" s="8">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>0.20548611111111112</v>
+      </c>
+      <c r="W18" s="32">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>82.505486111111111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="7">
         <f>B13+B12</f>
@@ -1471,10 +2484,52 @@
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="15"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R19" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S19" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T19" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U19" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V19" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W19" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B20" s="7">
         <f>B15+B14</f>
@@ -1493,14 +2548,786 @@
         <f>F15+F14</f>
         <v>62.5</v>
       </c>
+      <c r="J20" t="s">
+        <v>32</v>
+      </c>
+      <c r="L20" s="15"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S20" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T20" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U20" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V20" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W20" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>75</v>
+      </c>
+      <c r="L21" s="15"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q21" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R21" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S21" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T21" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U21" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V21" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W21" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="15"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q22" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R22" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S22" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T22" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U22" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V22" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W22" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="15"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q23" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R23" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S23" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T23" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U23" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V23" s="8" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W23" s="32" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" t="s">
+        <v>76</v>
+      </c>
+      <c r="L24" s="42"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="7" t="e">
+        <f>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q24" s="31" t="e">
+        <f>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R24" s="7" t="e">
+        <f>Table3[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S24" s="31" t="e">
+        <f>Table3[[#This Row],[ECPW]]-$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T24" s="7" t="e">
+        <f>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U24" s="31" t="e">
+        <f>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V24" s="10" t="e">
+        <f>Table3[[#This Row],[Mass + OH]]+$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W24" s="37" t="e">
+        <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W25" s="30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="L28" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="M28" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="N28" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="O28" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="P28" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q28" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="R28" t="s">
+        <v>61</v>
+      </c>
+      <c r="S28" t="s">
+        <v>96</v>
+      </c>
+      <c r="T28" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="U28" s="56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J29" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="K29" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="L29" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="M29" s="47">
+        <v>6.3E-2</v>
+      </c>
+      <c r="N29" s="46">
+        <v>104</v>
+      </c>
+      <c r="O29" s="46">
+        <v>4</v>
+      </c>
+      <c r="P29" s="7">
+        <f>M29/O29</f>
+        <v>1.575E-2</v>
+      </c>
+      <c r="Q29" s="31">
+        <f>N29/O29</f>
+        <v>26</v>
+      </c>
+      <c r="T29" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>4.7777777777777784E-3</v>
+      </c>
+      <c r="U29" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>26</v>
+      </c>
+      <c r="V29" s="57"/>
+      <c r="W29" s="57"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J30" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="L30" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="M30" s="41">
+        <v>0.05</v>
+      </c>
+      <c r="N30" s="40">
+        <v>880</v>
+      </c>
+      <c r="O30" s="40">
+        <v>2</v>
+      </c>
+      <c r="P30" s="7">
+        <f t="shared" ref="P30:P43" si="3">M30/O30</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Q30" s="31">
+        <f t="shared" ref="Q30:Q43" si="4">N30/O30</f>
+        <v>440</v>
+      </c>
+      <c r="T30" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>1.402777777777778E-2</v>
+      </c>
+      <c r="U30" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>440</v>
+      </c>
+      <c r="V30" s="57"/>
+      <c r="W30" s="57"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J31" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="40"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q31" s="31" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T31" s="7" t="e">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U31" s="31" t="e">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V31" s="57"/>
+      <c r="W31" s="57"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J32" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="28"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q32" s="31" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T32" s="7" t="e">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U32" s="31" t="e">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V32" s="57"/>
+      <c r="W32" s="57"/>
+    </row>
+    <row r="33" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J33" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="26"/>
+      <c r="L33" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="M33" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="N33" s="40">
+        <v>300</v>
+      </c>
+      <c r="O33" s="40">
+        <v>2</v>
+      </c>
+      <c r="P33" s="7">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q33" s="31">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="T33" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>8.9027777777777789E-2</v>
+      </c>
+      <c r="U33" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>150</v>
+      </c>
+      <c r="V33" s="57"/>
+      <c r="W33" s="57"/>
+    </row>
+    <row r="34" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J34" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="28"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q34" s="31" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T34" s="7" t="e">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U34" s="31" t="e">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V34" s="57"/>
+      <c r="W34" s="57"/>
+    </row>
+    <row r="35" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J35" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="26"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="40"/>
+      <c r="O35" s="40"/>
+      <c r="P35" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q35" s="31" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T35" s="7" t="e">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U35" s="31" t="e">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V35" s="57"/>
+      <c r="W35" s="57"/>
+    </row>
+    <row r="36" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J36" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" s="28"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q36" s="31" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T36" s="7" t="e">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U36" s="31" t="e">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V36" s="57"/>
+      <c r="W36" s="57"/>
+    </row>
+    <row r="37" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J37" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L37" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="M37" s="41">
+        <v>0.08</v>
+      </c>
+      <c r="N37" s="40">
+        <v>186</v>
+      </c>
+      <c r="O37" s="40">
+        <v>4</v>
+      </c>
+      <c r="P37" s="7">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="Q37" s="31">
+        <f t="shared" si="4"/>
+        <v>46.5</v>
+      </c>
+      <c r="T37" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="U37" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>46.5</v>
+      </c>
+      <c r="V37" s="57"/>
+      <c r="W37" s="57"/>
+    </row>
+    <row r="38" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J38" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="L38" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="M38" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="N38" s="40">
+        <v>300</v>
+      </c>
+      <c r="O38" s="40">
+        <v>2</v>
+      </c>
+      <c r="P38" s="7">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q38" s="31">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="T38" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>8.9027777777777789E-2</v>
+      </c>
+      <c r="U38" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>150</v>
+      </c>
+      <c r="V38" s="57"/>
+      <c r="W38" s="57"/>
+    </row>
+    <row r="39" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J39" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="K39" s="26"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q39" s="31" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T39" s="7" t="e">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U39" s="31" t="e">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V39" s="57"/>
+      <c r="W39" s="57"/>
+    </row>
+    <row r="40" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J40" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="K40" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="L40" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="M40" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="N40" s="40">
+        <v>300</v>
+      </c>
+      <c r="O40" s="40">
+        <v>2</v>
+      </c>
+      <c r="P40" s="7">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q40" s="31">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="T40" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>8.9027777777777789E-2</v>
+      </c>
+      <c r="U40" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>150</v>
+      </c>
+      <c r="V40" s="57"/>
+      <c r="W40" s="57"/>
+    </row>
+    <row r="41" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J41" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="26"/>
+      <c r="L41" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="M41" s="41">
+        <v>0.48</v>
+      </c>
+      <c r="N41" s="40">
+        <v>2700</v>
+      </c>
+      <c r="O41" s="40">
+        <v>2</v>
+      </c>
+      <c r="P41" s="7">
+        <f t="shared" si="3"/>
+        <v>0.24</v>
+      </c>
+      <c r="Q41" s="31">
+        <f t="shared" si="4"/>
+        <v>1350</v>
+      </c>
+      <c r="T41" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>0.22902777777777777</v>
+      </c>
+      <c r="U41" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>1350</v>
+      </c>
+      <c r="V41" s="57"/>
+      <c r="W41" s="57"/>
+    </row>
+    <row r="42" spans="10:23" x14ac:dyDescent="0.25">
+      <c r="J42" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="28"/>
+      <c r="L42" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="M42" s="41">
+        <v>0.48</v>
+      </c>
+      <c r="N42" s="40">
+        <v>1800</v>
+      </c>
+      <c r="O42" s="40">
+        <v>2</v>
+      </c>
+      <c r="P42" s="7">
+        <f t="shared" si="3"/>
+        <v>0.24</v>
+      </c>
+      <c r="Q42" s="31">
+        <f t="shared" si="4"/>
+        <v>900</v>
+      </c>
+      <c r="T42" s="7">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>0.22902777777777777</v>
+      </c>
+      <c r="U42" s="31">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>900</v>
+      </c>
+      <c r="V42" s="57"/>
+      <c r="W42" s="57"/>
+    </row>
+    <row r="43" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J43" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="L43" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="M43" s="41">
+        <v>0.2</v>
+      </c>
+      <c r="N43" s="40">
+        <v>300</v>
+      </c>
+      <c r="O43" s="40">
+        <v>2</v>
+      </c>
+      <c r="P43" s="7">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="Q43" s="31">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="R43" s="35">
+        <f t="shared" ref="R43" si="5">O43/P43</f>
+        <v>20</v>
+      </c>
+      <c r="S43" s="35">
+        <f t="shared" ref="S43" si="6">P43/Q43</f>
+        <v>6.6666666666666675E-4</v>
+      </c>
+      <c r="T43" s="27">
+        <f>Table4[[#This Row],[EMPW]]-$F$4</f>
+        <v>8.9027777777777789E-2</v>
+      </c>
+      <c r="U43" s="35">
+        <f>Table4[[#This Row],[ECPW]]</f>
+        <v>150</v>
+      </c>
+      <c r="V43" s="57"/>
+      <c r="W43" s="57"/>
     </row>
   </sheetData>
+  <sortState ref="J10:J24">
+    <sortCondition ref="J10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="4">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ballanced everything MechJeb and kOS intergration Having a problem with Radial resource switcher
</commit_message>
<xml_diff>
--- a/KSP Universal Storage 2.xlsx
+++ b/KSP Universal Storage 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\Kerbal Space Program 1.4 Making History\GameData\UniversalStorage2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D452CBBC-03B6-4B2D-B8A7-C990838C5965}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC13AB8E-3E69-4A37-8EC6-CF41862CA127}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="10590" windowHeight="12030" xr2:uid="{C3245EDE-D602-4B47-9FA3-AA7BA4BF5217}"/>
+    <workbookView xWindow="0" yWindow="3600" windowWidth="10590" windowHeight="12030" activeTab="1" xr2:uid="{C3245EDE-D602-4B47-9FA3-AA7BA4BF5217}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Mods list" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="109">
   <si>
     <t>Stock</t>
   </si>
@@ -332,6 +332,27 @@
   </si>
   <si>
     <t>Aerozine</t>
+  </si>
+  <si>
+    <t>EVA-X</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>2 Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electric </t>
   </si>
 </sst>
 </file>
@@ -341,7 +362,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +449,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -645,7 +673,7 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1"/>
@@ -722,6 +750,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Accent1" xfId="3" builtinId="29"/>
@@ -734,12 +765,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="7" builtinId="21"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -1132,10 +1166,10 @@
   <autoFilter ref="A9:F15" xr:uid="{E35C78EA-37D4-4ED3-9810-2F527211F7B1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A579DE4B-A322-4B2E-9837-103820C03232}" name="Part"/>
-    <tableColumn id="2" xr3:uid="{BDEA9424-295C-438D-BC3E-B712CD75D492}" name="Mass" dataDxfId="24" dataCellStyle="Input"/>
-    <tableColumn id="3" xr3:uid="{BEC8C509-96C0-4C1D-B987-D949FCD72522}" name="Cost" dataDxfId="23" dataCellStyle="Input"/>
+    <tableColumn id="2" xr3:uid="{BDEA9424-295C-438D-BC3E-B712CD75D492}" name="Mass" dataDxfId="25" dataCellStyle="Input"/>
+    <tableColumn id="3" xr3:uid="{BEC8C509-96C0-4C1D-B987-D949FCD72522}" name="Cost" dataDxfId="24" dataCellStyle="Input"/>
     <tableColumn id="4" xr3:uid="{2CDA1B83-518F-4FCE-B239-152F6AAB9B0E}" name="# Wedges"/>
-    <tableColumn id="5" xr3:uid="{D72B8143-BCE8-4CA0-92EB-4F25A654E009}" name="Mass PW" dataDxfId="22">
+    <tableColumn id="5" xr3:uid="{D72B8143-BCE8-4CA0-92EB-4F25A654E009}" name="Mass PW" dataDxfId="23">
       <calculatedColumnFormula>B10/D10</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{7C548BED-B2C0-48CA-8E75-2EE5E27D006C}" name="Cost PW">
@@ -1151,10 +1185,10 @@
   <autoFilter ref="A17:F20" xr:uid="{15374C48-326D-4B9F-89C7-9290C4904D94}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{EFC3A571-8606-4D34-9570-444E46172573}" name="Assembly" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{39B14A51-C030-4BF0-976E-6004D7CB7614}" name="Mass" dataDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{39B14A51-C030-4BF0-976E-6004D7CB7614}" name="Mass" dataDxfId="22" dataCellStyle="Normal"/>
     <tableColumn id="3" xr3:uid="{3085B6D2-8BD9-412D-9BB4-B061501AA3F5}" name="Cost" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{8AE4EF62-BE12-431E-8941-09FFEC2F04B1}" name="Column1" dataDxfId="20" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{07D0FC5F-9407-45B3-B1CF-2DA7FFBD07ED}" name="Mass PW" dataDxfId="19" dataCellStyle="Output"/>
+    <tableColumn id="4" xr3:uid="{8AE4EF62-BE12-431E-8941-09FFEC2F04B1}" name="Column1" dataDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{07D0FC5F-9407-45B3-B1CF-2DA7FFBD07ED}" name="Mass PW" dataDxfId="20" dataCellStyle="Output"/>
     <tableColumn id="6" xr3:uid="{EAED86FD-9C2D-43A3-8AED-2A35A4B0E8C1}" name="Cost PW" dataCellStyle="Output"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1168,31 +1202,31 @@
     <tableColumn id="1" xr3:uid="{D35C5EED-7BD1-4643-8282-F63E139564EA}" name="Wedge"/>
     <tableColumn id="6" xr3:uid="{8634F600-D183-4F35-9174-CF6AFDB437E9}" name="Resource"/>
     <tableColumn id="7" xr3:uid="{36D05634-ED80-4A39-A2B6-D12AE024D880}" name="Equivalent Part (EP)" dataCellStyle="Input"/>
-    <tableColumn id="8" xr3:uid="{3E6D94E4-6CE3-49EC-B2D7-CDEF9031A5D1}" name="EP Mass" dataDxfId="18" dataCellStyle="Input"/>
+    <tableColumn id="8" xr3:uid="{3E6D94E4-6CE3-49EC-B2D7-CDEF9031A5D1}" name="EP Mass" dataDxfId="19" dataCellStyle="Input"/>
     <tableColumn id="9" xr3:uid="{DB2B2C2C-9933-42E8-A081-7B51720E5BAE}" name="EP Cost" dataCellStyle="Input"/>
     <tableColumn id="10" xr3:uid="{7E87F25C-5A4C-4DF5-A29D-200B2970A86E}" name="EP Ratio" dataCellStyle="Input"/>
-    <tableColumn id="2" xr3:uid="{76FFECEC-42C1-4853-B453-CD67BCEA4C82}" name="EMPW" dataDxfId="17">
+    <tableColumn id="2" xr3:uid="{76FFECEC-42C1-4853-B453-CD67BCEA4C82}" name="EMPW" dataDxfId="18">
       <calculatedColumnFormula>Table3[[#This Row],[EP Mass]]/Table3[[#This Row],[EP Ratio]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6648A9CF-A240-4F40-9B6F-7036BFC6FDF0}" name="ECPW" dataDxfId="16">
+    <tableColumn id="3" xr3:uid="{6648A9CF-A240-4F40-9B6F-7036BFC6FDF0}" name="ECPW" dataDxfId="17">
       <calculatedColumnFormula>Table3[[#This Row],[EP Cost]]/Table3[[#This Row],[EP Ratio]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{335079E6-1470-4AD7-8DAE-D5030809B2E3}" name="Wedge Mass" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{335079E6-1470-4AD7-8DAE-D5030809B2E3}" name="Wedge Mass" dataDxfId="16">
       <calculatedColumnFormula>Table3[[#This Row],[EMPW]]-$F$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{99B210F1-A8A3-43A7-8333-E8BB85F0B547}" name="Wedge Cost" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{99B210F1-A8A3-43A7-8333-E8BB85F0B547}" name="Wedge Cost" dataDxfId="15">
       <calculatedColumnFormula>Table3[[#This Row],[ECPW]]-$F$5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{404FE096-C0F6-4430-B9AE-0C0079420A1E}" name="Mass + OH" dataDxfId="13">
+    <tableColumn id="11" xr3:uid="{404FE096-C0F6-4430-B9AE-0C0079420A1E}" name="Mass + OH" dataDxfId="14">
       <calculatedColumnFormula>Table3[[#This Row],[Wedge Mass]]+($F$4*$W$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{3E12FB57-74FA-4B05-ADFF-6CCFD7C06427}" name="Cost + OH" dataDxfId="12">
+    <tableColumn id="12" xr3:uid="{3E12FB57-74FA-4B05-ADFF-6CCFD7C06427}" name="Cost + OH" dataDxfId="13">
       <calculatedColumnFormula>Table3[[#This Row],[Wedge Cost]]+($F$4*$W$4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{59A654E4-65C3-446D-8823-21A7DAD93D58}" name="Mass with Structure" dataDxfId="11" dataCellStyle="Output">
+    <tableColumn id="13" xr3:uid="{59A654E4-65C3-446D-8823-21A7DAD93D58}" name="Mass with Structure" dataDxfId="12" dataCellStyle="Output">
       <calculatedColumnFormula>Table3[[#This Row],[Mass + OH]]+$F$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F355FCD9-68F4-49E3-835F-663E86D3B79B}" name="Cost with Structure" dataDxfId="10" dataCellStyle="Output">
+    <tableColumn id="14" xr3:uid="{F355FCD9-68F4-49E3-835F-663E86D3B79B}" name="Cost with Structure" dataDxfId="11" dataCellStyle="Output">
       <calculatedColumnFormula>Table3[[#This Row],[Cost + OH]]+$F$5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1204,25 +1238,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B3A231BC-39A7-4EE7-9404-BCFF8A0EB73D}" name="Table4" displayName="Table4" ref="J28:U43" totalsRowShown="0">
   <autoFilter ref="J28:U43" xr:uid="{46081FD9-DEF6-425C-B392-40ECBEDC37F3}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{3A5AB019-9F60-4DA4-846C-B79D4002996A}" name="Wedge" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{029965FB-BA4B-48F3-871C-0C2DCB8A6561}" name="Resource" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{038C1B73-CADE-41CD-B1C1-05FF0A2BE1CE}" name="Equivalent Part (EP)" dataDxfId="7" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{FD0E5793-2888-43BB-930B-A5077DC78A62}" name="EP Mass" dataDxfId="6" dataCellStyle="Input"/>
-    <tableColumn id="5" xr3:uid="{52F5C845-80EC-431F-8212-494C84B32728}" name="EP Cost" dataDxfId="5" dataCellStyle="Input"/>
-    <tableColumn id="6" xr3:uid="{AF154CBF-F54F-4E51-8889-F4DB73C16004}" name="EP Ratio" dataDxfId="4" dataCellStyle="Input"/>
-    <tableColumn id="7" xr3:uid="{6B1F7D26-131C-42E1-ABAF-EE8782299855}" name="EMPW" dataDxfId="3" dataCellStyle="Normal">
+    <tableColumn id="1" xr3:uid="{3A5AB019-9F60-4DA4-846C-B79D4002996A}" name="Wedge" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{029965FB-BA4B-48F3-871C-0C2DCB8A6561}" name="Resource" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{038C1B73-CADE-41CD-B1C1-05FF0A2BE1CE}" name="Equivalent Part (EP)" dataDxfId="8" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{FD0E5793-2888-43BB-930B-A5077DC78A62}" name="EP Mass" dataDxfId="7" dataCellStyle="Input"/>
+    <tableColumn id="5" xr3:uid="{52F5C845-80EC-431F-8212-494C84B32728}" name="EP Cost" dataDxfId="6" dataCellStyle="Input"/>
+    <tableColumn id="6" xr3:uid="{AF154CBF-F54F-4E51-8889-F4DB73C16004}" name="EP Ratio" dataDxfId="5" dataCellStyle="Input"/>
+    <tableColumn id="7" xr3:uid="{6B1F7D26-131C-42E1-ABAF-EE8782299855}" name="EMPW" dataDxfId="4" dataCellStyle="Normal">
       <calculatedColumnFormula>M29/O29</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B407898F-3ADA-4E54-ADDC-5EADD291509F}" name="ECPW" dataDxfId="2" dataCellStyle="Normal">
+    <tableColumn id="8" xr3:uid="{B407898F-3ADA-4E54-ADDC-5EADD291509F}" name="ECPW" dataDxfId="3" dataCellStyle="Normal">
       <calculatedColumnFormula>N29/O29</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{3F4CC5AE-B283-42BA-AA44-9D8055720245}" name="Column1"/>
     <tableColumn id="10" xr3:uid="{D9EFCA45-4D60-400B-AD7E-7C4B507FFC94}" name="Column2"/>
-    <tableColumn id="11" xr3:uid="{CED7D517-BD40-498E-AA55-203E544DE2AF}" name="Wedge Mass" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{CED7D517-BD40-498E-AA55-203E544DE2AF}" name="Wedge Mass" dataDxfId="2">
       <calculatedColumnFormula>Table4[[#This Row],[EMPW]]-$F$4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{37C9ED97-13F9-4DEF-BFA8-5B6D153D7855}" name="Wedge Cost" dataDxfId="1">
       <calculatedColumnFormula>Table4[[#This Row],[ECPW]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{25BB9756-D0BA-47AE-BB31-7B7BCD188B74}" name="Table5" displayName="Table5" ref="AA5:AB9" totalsRowShown="0">
+  <autoFilter ref="AA5:AB9" xr:uid="{D18E7AE5-F1BC-4CDA-8F1B-88F17E082B94}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{11B8B880-7890-4AA4-AB45-E7AA548EAC5E}" name="Resource"/>
+    <tableColumn id="2" xr3:uid="{830D2530-D43E-450C-A3F1-1965AFCD72D4}" name="TAC LS" dataDxfId="0">
+      <calculatedColumnFormula>AA6*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1526,10 +1573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A844A3D-DE41-49C6-9CA4-260D9D9B0D6E}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,9 +1594,10 @@
     <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>40</v>
@@ -1566,7 +1614,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1607,14 +1655,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
@@ -1623,125 +1671,138 @@
       <c r="J3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1755,10 +1816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1933BA2C-6D76-4E2A-A0F4-C7FFE13A3365}">
-  <dimension ref="A1:W43"/>
+  <dimension ref="A1:AF43"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V28" sqref="V28"/>
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,20 +1844,24 @@
     <col min="22" max="22" width="19" customWidth="1"/>
     <col min="23" max="23" width="20.85546875" customWidth="1"/>
     <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:32" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="24" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5"/>
+    <row r="3" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA3" s="58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>58</v>
       </c>
@@ -1814,7 +1879,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>59</v>
       </c>
@@ -1831,16 +1896,44 @@
       <c r="W5" s="36">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="21" x14ac:dyDescent="0.35">
+      <c r="AA5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AA7" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB7" s="60">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>63</v>
       </c>
       <c r="W8" s="55" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA8" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1901,8 +1994,17 @@
       <c r="W9" s="54" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB9" s="60">
+        <v>1250</v>
+      </c>
+      <c r="AD9">
+        <v>2.9249999999424001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1974,7 +2076,7 @@
         <v>37.505486111111111</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2044,7 +2146,7 @@
         <v>440.00548611111111</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2108,7 +2210,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2169,7 +2271,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2229,8 +2331,20 @@
         <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2290,8 +2404,28 @@
         <f>Table3[[#This Row],[Cost + OH]]+$F$5</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AA15" s="59">
+        <v>1.4166666666667001E-2</v>
+      </c>
+      <c r="AB15" s="60"/>
+      <c r="AC15" s="60">
+        <f>AA15*60</f>
+        <v>0.85000000000002007</v>
+      </c>
+      <c r="AD15" s="60">
+        <f>AC15*60</f>
+        <v>51.000000000001208</v>
+      </c>
+      <c r="AE15" s="60">
+        <f>AD15*24</f>
+        <v>1224.0000000000291</v>
+      </c>
+      <c r="AF15" s="60">
+        <f>AE15*2</f>
+        <v>2448.0000000000582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>7</v>
       </c>
@@ -3323,11 +3457,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>